<commit_message>
Completed creation of timeline from flight mission cycle
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeh2\OneDrive - University of Southampton\Documents\Southampton\GDP\General - Small Joint Implant Testing Rig\11 - Code\GDP_47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{F0530032-C7DE-42CC-9F26-CFB740CF3021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94651482-3D36-48B8-B93A-3727200A59F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>Light switch</t>
   </si>
   <si>
-    <t>Duration (s)</t>
-  </si>
-  <si>
     <t>Max_Force</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>Frequency_Angle</t>
+  </si>
+  <si>
+    <t>Duration</t>
   </si>
 </sst>
 </file>
@@ -436,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399F6792-B576-4406-B8DC-783C53DD3A12}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -506,22 +506,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -545,26 +545,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="76e0179195a8cd8c56075bbce18ec029">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ac947232578ced0354ff7668bd446e68" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -765,26 +745,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D638FD6-E65E-4C22-B18F-C675F10A950C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -801,4 +782,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated starting comments, Updated for new version of Pandas
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeh2\OneDrive - University of Southampton\Documents\Southampton\GDP\General - Small Joint Implant Testing Rig\11 - Code\GDP_47\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0C3B4EB-3393-45FF-8647-17DEA4F9DBF7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-2850" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Setting</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Typing</t>
   </si>
 </sst>
 </file>
@@ -434,10 +437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,6 +480,14 @@
         <v>50</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -487,7 +498,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed teh excel file to include knitting, was a sanity test for me!
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/hjc1g20_soton_ac_uk/Documents/Part 4/FEEG6013 - GDP/Electronics/GDP_47/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0C3B4EB-3393-45FF-8647-17DEA4F9DBF7}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B846F318-56DB-451C-AC13-D5AB68498AB0}"/>
   <bookViews>
-    <workbookView xWindow="-2850" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Setting</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Typing</t>
+  </si>
+  <si>
+    <t>Knitting</t>
   </si>
 </sst>
 </file>
@@ -429,7 +432,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -437,18 +440,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,7 +459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -464,7 +467,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -472,7 +475,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -480,12 +483,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5">
         <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -495,24 +506,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399F6792-B576-4406-B8DC-783C53DD3A12}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,19 +546,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -757,15 +773,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
@@ -774,6 +781,15 @@
     <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -796,14 +812,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -812,4 +820,12 @@
     <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Code working for Force-Time graph
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0C3B4EB-3393-45FF-8647-17DEA4F9DBF7}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A74AAFF-40BE-469B-B4CC-36E67C8340B4}"/>
   <bookViews>
-    <workbookView xWindow="-2850" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
     <sheet name="Flight Mission Cycle" sheetId="2" r:id="rId2"/>
-    <sheet name="Settings" sheetId="3" r:id="rId3"/>
+    <sheet name="Writing" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Setting</t>
   </si>
@@ -52,28 +52,13 @@
     <t>Light switch</t>
   </si>
   <si>
-    <t>Max_Force</t>
-  </si>
-  <si>
-    <t>Min_Force</t>
-  </si>
-  <si>
-    <t>Frequency_Force</t>
-  </si>
-  <si>
-    <t>Max_Angle</t>
-  </si>
-  <si>
-    <t>Min_Angle</t>
-  </si>
-  <si>
-    <t>Frequency_Angle</t>
-  </si>
-  <si>
     <t>Duration</t>
   </si>
   <si>
     <t>Typing</t>
+  </si>
+  <si>
+    <t>Force_End</t>
   </si>
 </sst>
 </file>
@@ -439,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -453,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -482,7 +467,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>60</v>
@@ -494,60 +479,55 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399F6792-B576-4406-B8DC-783C53DD3A12}">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADEC46F-0895-4F6B-9824-3972CAD06C20}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>20</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+      <c r="E3">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -556,6 +536,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a11b574cf4cb561680bfe1361c430e3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89de1c0a460d57237c269f87d1a77e15" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -784,39 +784,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2702E339-BBA0-4620-834D-3FDA04B7FF90}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -825,4 +793,31 @@
     <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2702E339-BBA0-4620-834D-3FDA04B7FF90}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added range of motion display
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A74AAFF-40BE-469B-B4CC-36E67C8340B4}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEA0C23-9270-4143-830C-C9E5CDAF1B10}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Setting</t>
   </si>
@@ -59,6 +59,15 @@
   </si>
   <si>
     <t>Force_End</t>
+  </si>
+  <si>
+    <t>Max_RoM</t>
+  </si>
+  <si>
+    <t>Min_RoM</t>
+  </si>
+  <si>
+    <t>Period</t>
   </si>
 </sst>
 </file>
@@ -480,10 +489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADEC46F-0895-4F6B-9824-3972CAD06C20}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,12 +500,12 @@
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -512,8 +521,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -528,6 +540,33 @@
       </c>
       <c r="E3">
         <v>25</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed errors, added error warnings
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7FEA0C23-9270-4143-830C-C9E5CDAF1B10}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42BC7078-9650-4936-96CE-89FDDC4FFCE4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView minimized="1" xWindow="-2940" yWindow="-16200" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>Typing</t>
   </si>
   <si>
-    <t>Force_End</t>
-  </si>
-  <si>
     <t>Max_RoM</t>
   </si>
   <si>
@@ -68,6 +65,9 @@
   </si>
   <si>
     <t>Period</t>
+  </si>
+  <si>
+    <t>Force</t>
   </si>
 </sst>
 </file>
@@ -492,7 +492,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +507,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -547,7 +547,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>-20</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -575,26 +575,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a11b574cf4cb561680bfe1361c430e3c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89de1c0a460d57237c269f87d1a77e15" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -823,26 +803,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2702E339-BBA0-4620-834D-3FDA04B7FF90}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -859,4 +840,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated cycle script to have fucntions and work for all settings. Added error detection.
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55B9FFC6-417A-4F9A-9532-DC03B0DB8C44}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FDC2F75-6A33-444F-AB3B-4A7FD5A63979}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
     <sheet name="Flight Mission Cycle" sheetId="2" r:id="rId2"/>
-    <sheet name="Writing" sheetId="4" r:id="rId3"/>
+    <sheet name="Typing" sheetId="7" r:id="rId3"/>
+    <sheet name="Light switch" sheetId="6" r:id="rId4"/>
+    <sheet name="Piano" sheetId="5" r:id="rId5"/>
+    <sheet name="Writing" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
   <si>
     <t>Setting</t>
   </si>
@@ -47,9 +50,6 @@
   </si>
   <si>
     <t>Piano</t>
-  </si>
-  <si>
-    <t>Light switch</t>
   </si>
   <si>
     <t>Duration</t>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +447,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,31 +455,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -488,11 +464,227 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>30</v>
+      </c>
+      <c r="D3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C66F4A08-766D-4199-A7AF-6FAC79FAE8C9}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F28E5F9-7560-4700-BC16-43CF6FD42907}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>30</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>30</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADEC46F-0895-4F6B-9824-3972CAD06C20}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +699,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -527,7 +719,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -547,7 +739,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>50</v>
@@ -555,7 +747,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>-20</v>
@@ -563,7 +755,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -575,8 +767,28 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a11b574cf4cb561680bfe1361c430e3c">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="89de1c0a460d57237c269f87d1a77e15" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
     <xsd:import namespace="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
     <xsd:element name="properties">
@@ -598,6 +810,7 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -660,6 +873,11 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="19" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="22" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -803,28 +1021,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2702E339-BBA0-4620-834D-3FDA04B7FF90}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -840,23 +1057,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Now gets total duration from summing each setting
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac.sharepoint.com/teams/SmallJointImplantTestingRig/Shared Documents/General/11 - Code/GDP_47/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FDC2F75-6A33-444F-AB3B-4A7FD5A63979}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{61BC9EDB-62EA-46B3-812F-EC1356CBC4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B8E830E-D37E-4CF7-B433-2D87AA1B08BB}"/>
   <bookViews>
-    <workbookView xWindow="1650" yWindow="16080" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Setting</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Force</t>
+  </si>
+  <si>
+    <t>Light switch</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,10 +455,35 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <f>SUM(Typing!B3:D3)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B5">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -468,7 +496,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +555,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -540,7 +568,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,10 +582,16 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -593,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F28E5F9-7560-4700-BC16-43CF6FD42907}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,7 +689,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -684,7 +718,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,6 +801,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
@@ -775,15 +818,6 @@
     <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1022,20 +1056,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
     <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Angle working with cycles - needs editting
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeh2\OneDrive - University of Southampton\Documents\Southampton\GDP\General - Small Joint Implant Testing Rig\11 - Code\GDP_47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9678E44-7F61-4968-BA10-08C4085554EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952F9CB8-1392-48D4-8FD5-19F31B3AFFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,13 +527,13 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>30</v>
       </c>
       <c r="D3">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -557,7 +557,7 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added light layout to to make labels visible
</commit_message>
<xml_diff>
--- a/Flight_Mission_Cycle.xlsx
+++ b/Flight_Mission_Cycle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joeh2\OneDrive - University of Southampton\Documents\Southampton\GDP\General - Small Joint Implant Testing Rig\11 - Code\GDP_47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952F9CB8-1392-48D4-8FD5-19F31B3AFFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43B4F40-E765-43F1-9A8D-784BFEF81CC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{DA22312A-0C2A-4384-9D35-840CD7FCF009}"/>
   </bookViews>
   <sheets>
     <sheet name="How to use" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A671B1A1-7FE6-4148-92D2-482FECAD7275}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF68743-A6F3-431E-B235-0E24B6BB11CE}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +541,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>-30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,7 +619,7 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>-30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>6</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -821,26 +821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010027F16B06E6E01148813C7ACA97AA34EF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa346ec97cd2b8cb95951b4135646f8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a58a784a-84fb-458e-a075-e295952a81e3" xmlns:ns3="685e9b33-d6f8-42eb-aee1-d32c251952d0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cdd15de96697d00dd4eeb440d71a501f" ns2:_="" ns3:_="">
     <xsd:import namespace="a58a784a-84fb-458e-a075-e295952a81e3"/>
@@ -1075,26 +1055,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a58a784a-84fb-458e-a075-e295952a81e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="685e9b33-d6f8-42eb-aee1-d32c251952d0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
-    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F12FEC0-8F9C-493A-8210-061C1FAC29C6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1111,4 +1092,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6C7064E-D01D-4C28-8C28-492E65D40FAD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a58a784a-84fb-458e-a075-e295952a81e3"/>
+    <ds:schemaRef ds:uri="685e9b33-d6f8-42eb-aee1-d32c251952d0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4EB332-C92E-41ED-8CB6-874A3DC7E696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>